<commit_message>
Added CreateCardTest class to test the CreateCard class, and added the Test Case to the excel sheet
</commit_message>
<xml_diff>
--- a/Test Cases/TestCase.xlsx
+++ b/Test Cases/TestCase.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Courses\Semester 4.2\Design Patterns\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Expected Result</t>
   </si>
@@ -158,6 +153,36 @@
   </si>
   <si>
     <t>OS: Windows 8.1                   IDE: Eclipse</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the CreateCard class creates both a Debit and Credit Card.  </t>
+  </si>
+  <si>
+    <t>1. User knows what kind of Card they want to create.</t>
+  </si>
+  <si>
+    <t>1. First Create a Instance of a Card.          2. Create a Debit Card using the instance.                                                     3. Create a Credit Card using the same instance.</t>
+  </si>
+  <si>
+    <t>1. New DebitCard object with name Tyler Test                 2. New CreditCard object with name Tyler Test</t>
+  </si>
+  <si>
+    <t>1. First created was the Debit Card so a message that A Debit Card has been created should show.     2. The Credit Card is created after and a message that A Credit Card has been created should be displayed.</t>
+  </si>
+  <si>
+    <t>1. If the type of card is correctly input, the result should be as expected.                             2. If a type of card does not exist, an error message is displayed saying card cannot be created.</t>
+  </si>
+  <si>
+    <t>Create Card Test Case</t>
+  </si>
+  <si>
+    <t>Tyler Serio</t>
+  </si>
+  <si>
+    <t>03/24/2015</t>
   </si>
 </sst>
 </file>
@@ -490,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -651,7 +676,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +798,56 @@
         <v>41</v>
       </c>
     </row>
+    <row r="3" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>26</v>
@@ -783,5 +858,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created the CreateAccountTest to test if both Savingsa nd Chequings will work. Also updated the Excel sheet to include the updated Test Case.
</commit_message>
<xml_diff>
--- a/Test Cases/TestCase.xlsx
+++ b/Test Cases/TestCase.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>Expected Result</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date of Execution </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>1. If the specified amount is within the limit, the result is as expected.
@@ -183,6 +180,30 @@
   </si>
   <si>
     <t>03/24/2015</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Verify that an account can be created for either Savings or Chequing</t>
+  </si>
+  <si>
+    <t>1. User knows what kind of account they want to createq</t>
+  </si>
+  <si>
+    <t>1. Cretae a Savings Account using the createAcc() method of CreateAccount class                                                         2. Create a Chequing Account using the createAcc() method of CreateAccount class</t>
+  </si>
+  <si>
+    <t>1. A New Savings Account object is created.                   2. A New Chequings Account object Is created.</t>
+  </si>
+  <si>
+    <t>Create Accounts Test Case</t>
+  </si>
+  <si>
+    <t>1. If a Savings Account is created, a message saying a Savings Account has been created should display.                                                                        2. If a Chequings Account is created, a message saying a Chequings Account has been created should display.</t>
+  </si>
+  <si>
+    <t>1. If Savings or Chequing is inserted for card type, the result is as specified.                           2. If a user doesn’t enter one of these two accounts, an error message telling them that type of account doesn’t exist will be displayed.</t>
   </si>
 </sst>
 </file>
@@ -675,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,107 +771,152 @@
     </row>
     <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>26</v>
+      <c r="N4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added AccountTest to see if the deposit method works. Updated the Test Case excel to add new case
</commit_message>
<xml_diff>
--- a/Test Cases/TestCase.xlsx
+++ b/Test Cases/TestCase.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>Expected Result</t>
   </si>
@@ -204,6 +204,27 @@
   </si>
   <si>
     <t>1. If Savings or Chequing is inserted for card type, the result is as specified.                           2. If a user doesn’t enter one of these two accounts, an error message telling them that type of account doesn’t exist will be displayed.</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Verify that funds can be desposted into an account.</t>
+  </si>
+  <si>
+    <t>1.User has created an account, either chequings or savings.</t>
+  </si>
+  <si>
+    <t>1. Create an account. Either chequings or savings.                                                 2. Run the deposit() method of the account and insert an amount                  3. Make sure the amount is equal to what should have been deposited.</t>
+  </si>
+  <si>
+    <t>1. A new Savings account object is created.                   2. A depost of 50 is made into the account.</t>
+  </si>
+  <si>
+    <t>1. If the depost is successful, a message letting you know that you have deposited the amount should be seen.                                                           2. If you enter a number less or equal to zero, an error message will be displayed.</t>
+  </si>
+  <si>
+    <t>1. If the depost is made successfully, the balance should be equal to 50 and no error message displayed.                                             2. If thedeposit in unsuccessful, the user is notified of the mistake in balance.</t>
   </si>
 </sst>
 </file>
@@ -696,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,6 +940,56 @@
         <v>40</v>
       </c>
     </row>
+    <row r="5" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="2"/>
     </row>

</xml_diff>

<commit_message>
Created Account Test Number 2 to make sure that a withdrawal on an account will work. Fixed the TransactionFeeState class to fix the withdrawl error by switching the if statement clause to be less than, not greater than. Updated the Test Case excel sheet and added new test case
</commit_message>
<xml_diff>
--- a/Test Cases/TestCase.xlsx
+++ b/Test Cases/TestCase.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>Expected Result</t>
   </si>
@@ -191,9 +191,6 @@
     <t>1. User knows what kind of account they want to createq</t>
   </si>
   <si>
-    <t>1. Cretae a Savings Account using the createAcc() method of CreateAccount class                                                         2. Create a Chequing Account using the createAcc() method of CreateAccount class</t>
-  </si>
-  <si>
     <t>1. A New Savings Account object is created.                   2. A New Chequings Account object Is created.</t>
   </si>
   <si>
@@ -221,10 +218,31 @@
     <t>1. A new Savings account object is created.                   2. A depost of 50 is made into the account.</t>
   </si>
   <si>
-    <t>1. If the depost is successful, a message letting you know that you have deposited the amount should be seen.                                                           2. If you enter a number less or equal to zero, an error message will be displayed.</t>
-  </si>
-  <si>
-    <t>1. If the depost is made successfully, the balance should be equal to 50 and no error message displayed.                                             2. If thedeposit in unsuccessful, the user is notified of the mistake in balance.</t>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Verify that funds can be withdrawn from an account.</t>
+  </si>
+  <si>
+    <t>1. Create an account. Either chequings or savings.                                                 2. Run the withdraw() method of the account and insert an amount                  3. Make sure the balance is equal to what should be after withdrawl and fees (if applicable)</t>
+  </si>
+  <si>
+    <t>1. A new Savings account object is created.                   2. A depost of 50 is made into the account.                   3. A withdrawl of 25 is made.</t>
+  </si>
+  <si>
+    <t>1. If the withdrawl is successful, a message letting you know that you have withdrawn the amount should be seen.                                                           2. If you enter a number that si greater than the balance, an error will be posted.</t>
+  </si>
+  <si>
+    <t>1. If the deposit is successful, a message letting you know that you have deposited the amount should be seen.                                                           2. If you enter a number less or equal to zero, an error message will be displayed.</t>
+  </si>
+  <si>
+    <t>1. Create a Savings Account using the createAcc() method of CreateAccount class                                                         2. Create a Chequing Account using the createAcc() method of CreateAccount class</t>
+  </si>
+  <si>
+    <t>1. If the withdrawl is made successfully, the balance should be equal to 23 and no error message displayed.                                             2. If the withdrawl is unsuccessful, the user is notified of the mistake in balance.</t>
+  </si>
+  <si>
+    <t>1. If the deposit is made successfully, the balance should be equal to 50 and no error message displayed.                                             2. If the deposit is unsuccessful, the user is notified of the mistake in balance.</t>
   </si>
 </sst>
 </file>
@@ -717,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -907,22 +925,22 @@
         <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>49</v>
@@ -945,34 +963,34 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>49</v>
@@ -987,6 +1005,56 @@
         <v>31</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>